<commit_message>
More questions/better img rendering
</commit_message>
<xml_diff>
--- a/TestEngine/www/ANSWERS.xlsx
+++ b/TestEngine/www/ANSWERS.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="267">
   <si>
     <t>ANSWER</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>any value</t>
+  </si>
+  <si>
+    <t>the file format for files that are stores in the library.</t>
   </si>
   <si>
     <t>the version of SAS that you are using.</t>
@@ -364,7 +367,585 @@
     <t>Some data values weren't appropriate for the SAS statements that you specified.</t>
   </si>
   <si>
-    <t>the file format for files that are stored in the library.</t>
+    <t>proc print data=flights.laguardia noobs;
+var on changes flight;
+where on &gt;=160;
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=flights.laguardia;
+var date on changed flight;
+where changed&gt;3;
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=flights.laguardia label; 
+id date;
+var boarded transferred flight;
+label boarded='On' transferred = 'Changed';
+where flight='219';
+run;</t>
+  </si>
+  <si>
+    <t>proc print flights.laguardia noobs;
+id date;
+var date on changed flight;
+where flight='219';
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=allsales.totals label;
+label region8='Region 8 Yearly Totals';
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=allsales.totals;
+label region8='Region 8 Yearly Totals';
+run;</t>
+  </si>
+  <si>
+    <t>proc print data allsales.totals label noobs;
+run;</t>
+  </si>
+  <si>
+    <t>proc print allsales.totals label;
+run;</t>
+  </si>
+  <si>
+    <t>where style='RANCH' or 'SPLIT' or 'TWOSTORY';</t>
+  </si>
+  <si>
+    <t>where style in 'RANCH' or 'SPLIT' or 'TWOSTORY';</t>
+  </si>
+  <si>
+    <t>where style in (RANCH, SPLIT, TWOSTORY);</t>
+  </si>
+  <si>
+    <t>where style in ('RANCH', 'SPLIT', 'TWOSTORY')</t>
+  </si>
+  <si>
+    <t>proc sort data=work.calc out=finance.dividend;
+run;</t>
+  </si>
+  <si>
+    <t>proc sort dividend out=calc;
+by account;
+run;</t>
+  </si>
+  <si>
+    <t>proc sort data=finance.dividend out=work.calc;
+by account;
+run;</t>
+  </si>
+  <si>
+    <t>proc sort from finance.dividend to calc;
+by account;
+run;</t>
+  </si>
+  <si>
+    <t>the DATE system option and the LABEL option in PROC PRINT</t>
+  </si>
+  <si>
+    <t>the DATE and NONUMBER system options and the DOUBLE and NOOBS options in PROC PRINT</t>
+  </si>
+  <si>
+    <t>the DATE and NONUMBERS system options and the DOUBLE option in PROC PRINT</t>
+  </si>
+  <si>
+    <t>the DATE and NONUMBER system options and the NOOBS option in PROC PRINT</t>
+  </si>
+  <si>
+    <t>var month instructors;
+sum instructors aerclass walkjogrun swim;</t>
+  </si>
+  <si>
+    <t>var month;
+sum instructors aerclass walkjogrun swim;</t>
+  </si>
+  <si>
+    <t>var month instructors aerclass;
+sum instructors aerclass walkjogrun swim;</t>
+  </si>
+  <si>
+    <t>The PROC PRINT step runs successfully, printing observations in their sorted order.</t>
+  </si>
+  <si>
+    <t>The PROC SORT step permanently sorts the input data set.</t>
+  </si>
+  <si>
+    <t>The PROC SORT step generates errors and stops processing, but the PROC PRINT step runs successful, printing observations in their original (unsorted) order.</t>
+  </si>
+  <si>
+    <t>The PROC SORT step runs successfully, but the PROC PRINT step generates errors and stops processing.</t>
+  </si>
+  <si>
+    <t>where amount &lt;= 5000 and 
+account = '101-1092' or rate = 0.095;</t>
+  </si>
+  <si>
+    <t>where (amount le 5000 and account='101-1092')
+or rate = 0.095;</t>
+  </si>
+  <si>
+    <t>where amounts &lt;=5000 and 
+(accounts ='101-1092' or rate eq 0.095);</t>
+  </si>
+  <si>
+    <t>where amount &lt;=5000 or accounts='101-1092'
+and rate = 0.095;</t>
+  </si>
+  <si>
+    <t>PROC PRINT displays all observations and variables in the data set. If you want an additional column for observation numbers, you can request it.</t>
+  </si>
+  <si>
+    <t>PROC PRINT displays columns in the following order: a column for observations numbers, all character variables, all numeric variables.</t>
+  </si>
+  <si>
+    <t>PROC PRINT displays all observations and variables in the data set, a column for observation numbers on the far left, and variables in the order in which they occur in the data set.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>25 observations, 4 variables</t>
+  </si>
+  <si>
+    <t>75 observations, 3 variables</t>
+  </si>
+  <si>
+    <t>75 observations, 4 variables</t>
+  </si>
+  <si>
+    <t>The options apply to all output data sets created in the DATA statement</t>
+  </si>
+  <si>
+    <t>Using the options with input data affects the content of the program data vector.</t>
+  </si>
+  <si>
+    <t>When the options are used in the same DATA step that includes a DROP or KEEP statement, the options are applied first.</t>
+  </si>
+  <si>
+    <t>If you don't need all the variables in your input data for processing, it's most efficient to eliminate them using one of these data set options in the DATA statement.</t>
+  </si>
+  <si>
+    <t>Month, Sport, Coach</t>
+  </si>
+  <si>
+    <t>Sport, Coach</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>data stresstest (drop=timemin timesec);
+set physical;
+TotalTime=(Timemin*60)+Timesec;
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=stressdata;
+label TotalTime='Duration of Test';
+drop TimeMine;
+run;</t>
+  </si>
+  <si>
+    <t>proc print data=stresstest (keep=TotalTime TimeMin);
+label TotalTime='Duration of Test';
+format TimeMin 5.2;
+run;</t>
+  </si>
+  <si>
+    <t>data fastorder(drop=Ordertime);
+set july.orders(keep=Product Units Price);
+if Ordertime&lt;4;
+Total=Units*Price;
+run;</t>
+  </si>
+  <si>
+    <t>data orders(drop=Ordertime);
+set july.fastorder(keep=Product Units Price);
+if Ordertime&lt;4;
+Total=Units*Price;
+run;</t>
+  </si>
+  <si>
+    <t>data fastorder(drop=Ordertime);
+set july.orders(keep=Product Units Price Ordertime);
+if Ordertime&lt;4;
+Total=Units*Price;
+run;</t>
+  </si>
+  <si>
+    <t>select region;
+when (2,3,5) output tropical;
+otherwise;
+end;</t>
+  </si>
+  <si>
+    <t>select;
+when (region=2,3,5) output tropical;
+otherwise;
+end;</t>
+  </si>
+  <si>
+    <t>select(region);
+when (2,3,5) output tropical;
+otherwise;
+end;</t>
+  </si>
+  <si>
+    <t>Because the OUTPUT statement does not specify a data set, both output data sets are empty.</t>
+  </si>
+  <si>
+    <t>All observations in the flora data set are written to both output data sets.</t>
+  </si>
+  <si>
+    <t>The DATA step writes the first observation to each output data set and then stops processing because no RETURN statement is specified</t>
+  </si>
+  <si>
+    <t>data mnthtot;
+set orion.aprsales;
+retain Mnth2Date;
+Mth2Dte=Mth2Dte+SaleAmt;
+run;</t>
+  </si>
+  <si>
+    <t>data mnthtot;
+set orion.aprsales;
+retain Mth2Dte 0;
+Mth2Dte=Mth2Dte+SaleAmt;
+run;</t>
+  </si>
+  <si>
+    <t>Total_Retail_Price+Sales2Dte;</t>
+  </si>
+  <si>
+    <t>Sales2Dte+Total_Retail_Price;</t>
+  </si>
+  <si>
+    <t>Sales2Dte=Sales2Dte+Total_Retail_Price</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>A change in the value of LAST.JobCode causes the value of LAST.Gender to change</t>
+  </si>
+  <si>
+    <t>A change in the value of LAST.Gender causes the value of LAST.JobCode to be set to 1</t>
+  </si>
+  <si>
+    <t>Both LAST.JobCode and LAST.Gender are stored in the new data set</t>
+  </si>
+  <si>
+    <t>The data sets listed in the SET statement must be indexed or sorted by the values of the BY variable(s)</t>
+  </si>
+  <si>
+    <t>The DATA step automatically creates two new variables, FIRST. And LAST., for each variables in the BY statement</t>
+  </si>
+  <si>
+    <t>The FIRST. And LAST. Variables identify the first and last observation in each BY group, respectively</t>
+  </si>
+  <si>
+    <t>The FIRST. And LAST. Variables have values of 0 when SAS is processing an observation with the first occurrence of a new value for those variables, and a value of 1 for the other observations.</t>
+  </si>
+  <si>
+    <t>FIRST.BY-variable=0 LAST.BY-variable=0</t>
+  </si>
+  <si>
+    <t>FIRST.BY-variable=1 LAST.BY-variable=0</t>
+  </si>
+  <si>
+    <t>FIRST.BY-variable=1 LAST.BY-variable=1</t>
+  </si>
+  <si>
+    <t>FIRST.BY-variable=0 LAST.BY-variable=1</t>
+  </si>
+  <si>
+    <t>Output the first observation of each BY group.</t>
+  </si>
+  <si>
+    <t>Set the accumulating variable to zero at the start of each BY group.</t>
+  </si>
+  <si>
+    <t>Increment the accumulating variable with a sum statement (automatically retains).</t>
+  </si>
+  <si>
+    <t>if first.jobtype;</t>
+  </si>
+  <si>
+    <t>if last.jobtype;</t>
+  </si>
+  <si>
+    <t>if first.jobtype then output;</t>
+  </si>
+  <si>
+    <t>if last.jobtype then output=1;</t>
+  </si>
+  <si>
+    <t>column input</t>
+  </si>
+  <si>
+    <t>formatted input</t>
+  </si>
+  <si>
+    <t>a and b</t>
+  </si>
+  <si>
+    <t>!n'</t>
+  </si>
+  <si>
+    <t>+n'</t>
+  </si>
+  <si>
+    <t>#n'</t>
+  </si>
+  <si>
+    <t>@n'</t>
+  </si>
+  <si>
+    <t>standard free-format data</t>
+  </si>
+  <si>
+    <t>standard data in fixed fields</t>
+  </si>
+  <si>
+    <t>nonstandard data in fixed fields</t>
+  </si>
+  <si>
+    <t>input Item $9. @20 Quantity 3.;</t>
+  </si>
+  <si>
+    <t>input Item $9. +11 Quantity 3.;</t>
+  </si>
+  <si>
+    <t>input Item $9. +10 Quantity 3.;</t>
+  </si>
+  <si>
+    <t>input @14 Fname $10. @1 Lname $10./
+Department $7./
+Salary comma10.;</t>
+  </si>
+  <si>
+    <t>input @14 Fname $10. @1 Lname $10.
+#2 Department $7.
+#3 Salary comma10.;</t>
+  </si>
+  <si>
+    <t>both a and b</t>
+  </si>
+  <si>
+    <t>Load the next file in the input buffer.</t>
+  </si>
+  <si>
+    <t>Load the next field in the input buffer.</t>
+  </si>
+  <si>
+    <t>Load the next record in the input buffer.</t>
+  </si>
+  <si>
+    <t>The pointer position does not change.</t>
+  </si>
+  <si>
+    <t>No new record is loaded into the input buffer.</t>
+  </si>
+  <si>
+    <t>The next INPUT statement for the same iteration of the DATA step continues to read the same record.</t>
+  </si>
+  <si>
+    <t>State=scan(Address2,2);</t>
+  </si>
+  <si>
+    <t>State=scan(Address2,13,2);</t>
+  </si>
+  <si>
+    <t>State=substr(Address2,2);</t>
+  </si>
+  <si>
+    <t>State=substr(Address2,13,2);</t>
+  </si>
+  <si>
+    <t>data work.piedmont(drop=AreaCode Exchange);
+set clients.piedmont;
+AreaCode=substr(Phone,1,3);
+Exchange=substr(Phone,5,3);
+if AreaCode='919' and Exchange='555' then Phone=substr('920',1,3);
+run;</t>
+  </si>
+  <si>
+    <t>data work.piedmont(drop=AreaCode Exchange);
+set clients.piedmont;
+AreaCode=substr(Phone,1,3);
+Exchange=substr(Phone,5,3);
+if AreaCode='919' and Exchange='555' then substr(Phone,1,3)='920';
+run;</t>
+  </si>
+  <si>
+    <t>data work.maillist;
+set retail.maillist;
+length FullName $ 40;
+FullName=trim(FirstName) || ' ' || LastName;
+run;</t>
+  </si>
+  <si>
+    <t>data work.maillist;
+set retail.maillist;
+length FullName $ 50;
+FullName=trim(FirstName|| ' ' ||LastName);
+run;</t>
+  </si>
+  <si>
+    <t>data work.bookcase;
+set furn.bookcase;
+if find(Finish,'walnut',I);
+run;</t>
+  </si>
+  <si>
+    <t>data work.bookcase;
+set furn.bookcase;
+if find(Finish,'walnut','I')&gt;0;
+run;</t>
+  </si>
+  <si>
+    <t>96701-006</t>
+  </si>
+  <si>
+    <t>HNL:</t>
+  </si>
+  <si>
+    <t>HNL:96701</t>
+  </si>
+  <si>
+    <t>1-006</t>
+  </si>
+  <si>
+    <t>New_Company=propcase(Company);</t>
+  </si>
+  <si>
+    <t>New_Company=propcase(Company, '&amp;');</t>
+  </si>
+  <si>
+    <t>New_Company=propcase(Company,' ,&amp;');</t>
+  </si>
+  <si>
+    <t>New_Company=propcase(Company,' &amp;');</t>
+  </si>
+  <si>
+    <t>ID=catx(State,Region,Area,'-');</t>
+  </si>
+  <si>
+    <t>ID=cat(State,Region,Area);</t>
+  </si>
+  <si>
+    <t>ID=catx('-',State,Region,Area);</t>
+  </si>
+  <si>
+    <t>ID=cats(State,Region,Area);</t>
+  </si>
+  <si>
+    <t>Name=transwrd(Name,"MISS","MS.");</t>
+  </si>
+  <si>
+    <t>Name=tranwrd(Name,"MS.","MISS");</t>
+  </si>
+  <si>
+    <t>Name=tranwrd(Name,"MISS","MS.");</t>
+  </si>
+  <si>
+    <t>3 blanks</t>
+  </si>
+  <si>
+    <t>mean(Var1,Var4)</t>
+  </si>
+  <si>
+    <t>mean(Var1-Var4)</t>
+  </si>
+  <si>
+    <t>mean(of Var1,Var4)</t>
+  </si>
+  <si>
+    <t>mean(of Var1-Var4)</t>
+  </si>
+  <si>
+    <t>Total=sum(of Year1-Year4);</t>
+  </si>
+  <si>
+    <t>Total=sum(of Year2--Year4);</t>
+  </si>
+  <si>
+    <t>Total=sum(of Year:);</t>
+  </si>
+  <si>
+    <t>CEIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT </t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>Decrease=round(PctDec,1);</t>
+  </si>
+  <si>
+    <t>Decrease=ceil(PctDec);</t>
+  </si>
+  <si>
+    <t>Decrease=floor(PctDec);</t>
+  </si>
+  <si>
+    <t>Decrease=int(PctDec);</t>
+  </si>
+  <si>
+    <t>SAS converts the values of PayRate to numeric values. No message is written to the log.</t>
+  </si>
+  <si>
+    <t>SAS converts the values of PayRate to numeric values. A message is written to the log.</t>
+  </si>
+  <si>
+    <t>SAS converts the values of Hours to character values. A message is written to the log.</t>
+  </si>
+  <si>
+    <t>put(Level,3.)</t>
+  </si>
+  <si>
+    <t>input(3.,Level)</t>
+  </si>
+  <si>
+    <t>put(3.,Level)</t>
+  </si>
+  <si>
+    <t>input(Level,3.)</t>
+  </si>
+  <si>
+    <t>Location=Dept||'/'||put(SiteNum, $3);</t>
+  </si>
+  <si>
+    <t>Location=Dept||'/'||put(SiteNum,4);</t>
+  </si>
+  <si>
+    <t>Location=Dept||'/'||put(SiteNum,3.1);</t>
+  </si>
+  <si>
+    <t>Location=Dept||'/'||put(SiteNum,4.1);</t>
+  </si>
+  <si>
+    <t>put(comma10.2,Base)</t>
+  </si>
+  <si>
+    <t>put(Base,comma10.2)</t>
+  </si>
+  <si>
+    <t>input(Base,comma10.2)</t>
+  </si>
+  <si>
+    <t>input(comma10.2,Base)</t>
   </si>
 </sst>
 </file>
@@ -400,11 +981,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,8 +1294,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -986,19 +1571,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1006,19 +1591,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1026,19 +1611,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,19 +1631,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,19 +1651,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1086,19 +1671,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1106,19 +1691,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,19 +1711,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,19 +1731,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1166,19 +1751,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
         <v>81</v>
       </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" t="s">
-        <v>80</v>
-      </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1186,19 +1771,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,19 +1791,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
         <v>88</v>
       </c>
-      <c r="C25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" t="s">
-        <v>87</v>
-      </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1226,19 +1811,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1246,19 +1831,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,19 +1851,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
         <v>97</v>
       </c>
-      <c r="C28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" t="s">
-        <v>96</v>
-      </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,16 +1871,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
         <v>100</v>
       </c>
-      <c r="C29" t="s">
-        <v>99</v>
-      </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
         <v>23</v>
@@ -1306,347 +1891,1181 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" t="s">
         <v>103</v>
       </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>51</v>
+      </c>
+      <c r="C45">
+        <v>200</v>
+      </c>
+      <c r="D45">
+        <v>201</v>
+      </c>
+      <c r="E45">
+        <v>50</v>
+      </c>
+      <c r="F45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>130</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>100</v>
+      </c>
+      <c r="F51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>70</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>30</v>
+      </c>
+      <c r="F52">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>808</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D76">
+        <v>808</v>
+      </c>
+      <c r="E76">
+        <v>100</v>
+      </c>
+      <c r="F76">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>7</v>
+      </c>
+      <c r="D80">
+        <v>7.8</v>
+      </c>
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>

</xml_diff>